<commit_message>
Politique de tests et cahier de recette
Rédaction du cahier de recette et de la politique de test avec les tests
unitaires.
</commit_message>
<xml_diff>
--- a/1- Documents ESGI/Réunions.xlsx
+++ b/1- Documents ESGI/Réunions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="0" windowWidth="25695" windowHeight="10785"/>
+    <workbookView xWindow="4515" yWindow="0" windowWidth="25695" windowHeight="10785"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
   <si>
     <t>Damien</t>
   </si>
@@ -48,7 +48,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,8 +86,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +122,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -216,13 +228,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
@@ -233,6 +246,16 @@
     <xf numFmtId="14" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -254,11 +277,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
@@ -548,7 +569,7 @@
   <dimension ref="A3:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,10 +582,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="7">
         <v>42353</v>
       </c>
@@ -578,7 +599,7 @@
         <v>42006</v>
       </c>
       <c r="G3" s="7">
-        <v>42008</v>
+        <v>42007</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -586,13 +607,15 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10" t="s">
+        <v>5</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="1"/>
@@ -601,13 +624,15 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="10" t="s">
+        <v>5</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="1"/>
@@ -616,13 +641,15 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="11" t="s">
+        <v>5</v>
+      </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="6"/>
@@ -631,23 +658,23 @@
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="15" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H7" s="1"/>

</xml_diff>